<commit_message>
fixed times in data sheets and fit parameters for cerio
</commit_message>
<xml_diff>
--- a/Daphnia_large_Feeding_Nov11.xlsx
+++ b/Daphnia_large_Feeding_Nov11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8365a1eecae1c53e/Documents/GitHub/PreliminaryExperiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="ABE17B3680291292351C4062EBC4717D49E907BD" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{101FE043-E15B-4F4A-810C-848248B089D8}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="ABE17B3680291292351C4062EBC4717D49E907BD" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{4AD67BA7-99C8-49DD-A802-158A20350351}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7635" xr2:uid="{D8B4E32F-DAC1-4B29-B0CB-C75E22676032}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Rep</t>
   </si>
@@ -74,11 +74,32 @@
   <si>
     <t>baby</t>
   </si>
+  <si>
+    <t>Chl_time_1</t>
+  </si>
+  <si>
+    <t>Nh4_time_1</t>
+  </si>
+  <si>
+    <t>Chl_time_2</t>
+  </si>
+  <si>
+    <t>Nh4_time_2</t>
+  </si>
+  <si>
+    <t>Chl_Time_Diff</t>
+  </si>
+  <si>
+    <t>Nh4_Time_Diff</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -104,12 +125,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,15 +464,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2E4590-0DC6-42F1-B25A-A63DDB570770}">
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:V41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" style="2" customWidth="1"/>
+    <col min="16" max="17" width="12.5703125" style="4" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,1824 +490,2622 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
       <c r="C2">
         <v>736</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="E2">
         <v>9.8740000000000006</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>746</v>
       </c>
-      <c r="F2">
+      <c r="G2" s="2">
+        <v>0.32361111111111113</v>
+      </c>
+      <c r="H2">
         <v>12.77</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>7.2</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>20.8</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>1335</v>
       </c>
-      <c r="J2">
+      <c r="L2" s="2">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="M2">
         <v>6.42</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>1340</v>
       </c>
-      <c r="L2">
+      <c r="O2" s="2">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="P2" s="4">
+        <f>HOUR(L2-D2)*60+ MINUTE(L2-D2)</f>
+        <v>359</v>
+      </c>
+      <c r="Q2" s="4">
+        <f>HOUR(O2-G2)*60+MINUTE(O2-G2)</f>
+        <v>354</v>
+      </c>
+      <c r="R2">
         <v>10.32</v>
       </c>
-      <c r="M2">
+      <c r="S2">
         <v>7.3</v>
       </c>
-      <c r="N2">
+      <c r="T2">
         <v>20.5</v>
       </c>
-      <c r="O2">
+      <c r="U2">
         <v>23</v>
       </c>
-      <c r="P2">
+      <c r="V2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
       <c r="C3">
         <v>743</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
+        <v>0.3215277777777778</v>
+      </c>
+      <c r="E3">
         <v>15.11</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>753</v>
       </c>
-      <c r="F3">
+      <c r="G3" s="2">
+        <v>0.32847222222222222</v>
+      </c>
+      <c r="H3">
         <v>14.9</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>7.3</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>20.8</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>1337</v>
       </c>
-      <c r="J3">
+      <c r="L3" s="2">
+        <v>0.56736111111111109</v>
+      </c>
+      <c r="M3">
         <v>3.4540000000000002</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>1342</v>
       </c>
-      <c r="L3">
+      <c r="O3" s="2">
+        <v>0.5708333333333333</v>
+      </c>
+      <c r="P3" s="4">
+        <f t="shared" ref="P3:P41" si="0">HOUR(L3-D3)*60+ MINUTE(L3-D3)</f>
+        <v>354</v>
+      </c>
+      <c r="Q3" s="4">
+        <f t="shared" ref="Q3:Q41" si="1">HOUR(O3-G3)*60+MINUTE(O3-G3)</f>
+        <v>349</v>
+      </c>
+      <c r="R3">
         <v>10.36</v>
       </c>
-      <c r="M3">
+      <c r="S3">
         <v>7.4</v>
       </c>
-      <c r="N3">
+      <c r="T3">
         <v>20.2</v>
       </c>
-      <c r="O3">
+      <c r="U3">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>23</v>
       </c>
       <c r="C4">
         <v>745</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="E4">
         <v>1.1579999999999999</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>804</v>
       </c>
-      <c r="F4">
+      <c r="G4" s="2">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="H4">
         <v>8.44</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>7.3</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>20</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>1339</v>
       </c>
-      <c r="J4">
+      <c r="L4" s="2">
+        <v>0.56874999999999998</v>
+      </c>
+      <c r="M4">
         <v>0.95399999999999996</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>1344</v>
       </c>
-      <c r="L4">
+      <c r="O4" s="2">
+        <v>0.57222222222222219</v>
+      </c>
+      <c r="P4" s="4">
+        <f t="shared" si="0"/>
+        <v>354</v>
+      </c>
+      <c r="Q4" s="4">
+        <f t="shared" si="1"/>
+        <v>340</v>
+      </c>
+      <c r="R4">
         <v>7.83</v>
       </c>
-      <c r="M4">
+      <c r="S4">
         <v>7.4</v>
       </c>
-      <c r="N4">
+      <c r="T4">
         <v>20.3</v>
       </c>
-      <c r="O4">
+      <c r="U4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>25</v>
       </c>
       <c r="C5">
         <v>751</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
+        <v>0.32708333333333334</v>
+      </c>
+      <c r="E5">
         <v>22.39</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>817</v>
       </c>
-      <c r="F5">
+      <c r="G5" s="2">
+        <v>0.34513888888888888</v>
+      </c>
+      <c r="H5">
         <v>13.53</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>7.4</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>19.8</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>1341</v>
       </c>
-      <c r="J5">
+      <c r="L5" s="2">
+        <v>0.57013888888888886</v>
+      </c>
+      <c r="M5">
         <v>2.9780000000000002</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>1355</v>
       </c>
-      <c r="L5">
+      <c r="O5" s="2">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" si="1"/>
+        <v>338</v>
+      </c>
+      <c r="R5">
         <v>13.63</v>
       </c>
-      <c r="M5">
+      <c r="S5">
         <v>7.4</v>
       </c>
-      <c r="N5">
+      <c r="T5">
         <v>19.8</v>
       </c>
-      <c r="O5">
+      <c r="U5">
         <v>22</v>
       </c>
-      <c r="P5">
+      <c r="V5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>35</v>
       </c>
       <c r="C6">
         <v>757</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
+        <v>0.33124999999999999</v>
+      </c>
+      <c r="E6">
         <v>2.984</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>820</v>
       </c>
-      <c r="F6">
+      <c r="G6" s="2">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="H6">
         <v>8.4499999999999993</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>7.3</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>19.7</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>1343</v>
       </c>
-      <c r="J6">
+      <c r="L6" s="2">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="M6">
         <v>1.4930000000000001</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>1357</v>
       </c>
-      <c r="L6">
+      <c r="O6" s="2">
+        <v>0.58124999999999993</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="0"/>
+        <v>346</v>
+      </c>
+      <c r="Q6" s="4">
+        <f t="shared" si="1"/>
+        <v>337</v>
+      </c>
+      <c r="R6">
         <v>8.83</v>
       </c>
-      <c r="M6">
+      <c r="S6">
         <v>7.4</v>
       </c>
-      <c r="N6">
+      <c r="T6">
         <v>20.3</v>
       </c>
-      <c r="O6">
+      <c r="U6">
         <v>17</v>
       </c>
-      <c r="P6">
+      <c r="V6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
       <c r="C7">
         <v>803</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="E7">
         <v>14.93</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>831</v>
       </c>
-      <c r="F7">
+      <c r="G7" s="2">
+        <v>0.35486111111111113</v>
+      </c>
+      <c r="H7">
         <v>11.44</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>7.4</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>19.8</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>1401</v>
       </c>
-      <c r="J7">
+      <c r="L7" s="2">
+        <v>0.58402777777777781</v>
+      </c>
+      <c r="M7">
         <v>5.95</v>
       </c>
-      <c r="K7">
+      <c r="N7">
         <v>1405</v>
       </c>
-      <c r="L7">
+      <c r="O7" s="2">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="0"/>
+        <v>358</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" si="1"/>
+        <v>334</v>
+      </c>
+      <c r="R7">
         <v>10.220000000000001</v>
       </c>
-      <c r="M7">
+      <c r="S7">
         <v>7.4</v>
       </c>
-      <c r="N7">
+      <c r="T7">
         <v>20</v>
       </c>
-      <c r="O7">
+      <c r="U7">
         <v>21</v>
       </c>
-      <c r="P7">
+      <c r="V7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>17</v>
       </c>
       <c r="C8">
         <v>808</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
+        <v>0.33888888888888885</v>
+      </c>
+      <c r="E8">
         <v>0.98099999999999998</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>838</v>
       </c>
-      <c r="F8">
+      <c r="G8" s="2">
+        <v>0.35972222222222222</v>
+      </c>
+      <c r="H8">
         <v>8.81</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>7.3</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>19.600000000000001</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>1402</v>
       </c>
-      <c r="J8">
+      <c r="L8" s="2">
+        <v>0.58472222222222225</v>
+      </c>
+      <c r="M8">
         <v>0.88700000000000001</v>
       </c>
-      <c r="K8">
+      <c r="N8">
         <v>1408</v>
       </c>
-      <c r="L8">
+      <c r="O8" s="2">
+        <v>0.58888888888888891</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="0"/>
+        <v>354</v>
+      </c>
+      <c r="Q8" s="4">
+        <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
+      <c r="R8">
         <v>8.19</v>
       </c>
-      <c r="M8">
+      <c r="S8">
         <v>7.3</v>
       </c>
-      <c r="N8">
+      <c r="T8">
         <v>20.100000000000001</v>
       </c>
-      <c r="O8">
+      <c r="U8">
         <v>23</v>
       </c>
-      <c r="P8">
+      <c r="V8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>27</v>
       </c>
       <c r="C9">
         <v>815</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
+        <v>0.34375</v>
+      </c>
+      <c r="E9">
         <v>23.93</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>852</v>
       </c>
-      <c r="F9">
+      <c r="G9" s="2">
+        <v>0.36944444444444446</v>
+      </c>
+      <c r="H9">
         <v>13.88</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>7.5</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>19.600000000000001</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>1404</v>
       </c>
-      <c r="J9">
+      <c r="L9" s="2">
+        <v>0.58611111111111114</v>
+      </c>
+      <c r="M9">
         <v>5.0640000000000001</v>
       </c>
-      <c r="K9">
+      <c r="N9">
         <v>1416</v>
       </c>
-      <c r="L9">
+      <c r="O9" s="2">
+        <v>0.59444444444444444</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="0"/>
+        <v>349</v>
+      </c>
+      <c r="Q9" s="4">
+        <f t="shared" si="1"/>
+        <v>324</v>
+      </c>
+      <c r="R9">
         <v>15.34</v>
       </c>
-      <c r="M9">
+      <c r="S9">
         <v>7.4</v>
       </c>
-      <c r="N9">
+      <c r="T9">
         <v>20</v>
       </c>
-      <c r="O9">
+      <c r="U9">
         <v>16</v>
       </c>
-      <c r="P9">
+      <c r="V9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>38</v>
       </c>
       <c r="C10">
         <v>818</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
+        <v>0.34583333333333338</v>
+      </c>
+      <c r="E10">
         <v>2.7120000000000002</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>900</v>
       </c>
-      <c r="F10">
+      <c r="G10" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="H10">
         <v>10.92</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>7.4</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>19.8</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>1406</v>
       </c>
-      <c r="J10">
+      <c r="L10" s="2">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="M10">
         <v>2.4969999999999999</v>
       </c>
-      <c r="K10">
+      <c r="N10">
         <v>1419</v>
       </c>
-      <c r="L10">
+      <c r="O10" s="2">
+        <v>0.59652777777777777</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+      <c r="Q10" s="4">
+        <f t="shared" si="1"/>
+        <v>319</v>
+      </c>
+      <c r="R10">
         <v>10.8</v>
       </c>
-      <c r="M10">
+      <c r="S10">
         <v>7.5</v>
       </c>
-      <c r="N10">
+      <c r="T10">
         <v>19.899999999999999</v>
       </c>
-      <c r="O10">
+      <c r="U10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="C11">
         <v>823</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="E11">
         <v>9.0340000000000007</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>905</v>
       </c>
-      <c r="F11">
+      <c r="G11" s="2">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="H11">
         <v>9.32</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>7.4</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>20.100000000000001</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>1408</v>
       </c>
-      <c r="J11">
+      <c r="L11" s="2">
+        <v>0.58888888888888891</v>
+      </c>
+      <c r="M11">
         <v>5.6139999999999999</v>
       </c>
-      <c r="K11">
+      <c r="N11">
         <v>1423</v>
       </c>
-      <c r="L11">
+      <c r="O11" s="2">
+        <v>0.59930555555555554</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" si="0"/>
+        <v>345</v>
+      </c>
+      <c r="Q11" s="4">
+        <f t="shared" si="1"/>
+        <v>318</v>
+      </c>
+      <c r="R11">
         <v>10.039999999999999</v>
       </c>
-      <c r="M11">
+      <c r="S11">
         <v>7.4</v>
       </c>
-      <c r="N11">
+      <c r="T11">
         <v>20</v>
       </c>
-      <c r="O11">
+      <c r="U11">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>18</v>
       </c>
       <c r="C12">
         <v>830</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E12">
         <v>0.89</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>914</v>
       </c>
-      <c r="F12">
+      <c r="G12" s="2">
+        <v>0.38472222222222219</v>
+      </c>
+      <c r="H12">
         <v>7.74</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>7.3</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>20.399999999999999</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>1430</v>
       </c>
-      <c r="J12">
+      <c r="L12" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="M12">
         <v>0.92700000000000005</v>
       </c>
-      <c r="K12">
+      <c r="N12">
         <v>1434</v>
       </c>
-      <c r="L12">
+      <c r="O12" s="2">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="1"/>
+        <v>320</v>
+      </c>
+      <c r="R12">
         <v>7.35</v>
       </c>
-      <c r="M12">
+      <c r="S12">
         <v>7.4</v>
       </c>
-      <c r="N12">
+      <c r="T12">
         <v>19.7</v>
       </c>
-      <c r="O12">
+      <c r="U12">
         <v>18</v>
       </c>
-      <c r="P12">
+      <c r="V12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>28</v>
       </c>
       <c r="C13">
         <v>835</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="E13">
         <v>22.41</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>924</v>
       </c>
-      <c r="F13">
+      <c r="G13" s="2">
+        <v>0.39166666666666666</v>
+      </c>
+      <c r="H13">
         <v>13.93</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>7.4</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>20.5</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>1432</v>
       </c>
-      <c r="J13">
+      <c r="L13" s="2">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="M13">
         <v>5.8760000000000003</v>
       </c>
-      <c r="K13">
+      <c r="N13">
         <v>1437</v>
       </c>
-      <c r="L13">
+      <c r="O13" s="2">
+        <v>0.60902777777777783</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="0"/>
+        <v>357</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="1"/>
+        <v>313</v>
+      </c>
+      <c r="R13">
         <v>14.6</v>
       </c>
-      <c r="M13">
+      <c r="S13">
         <v>7.5</v>
       </c>
-      <c r="N13">
+      <c r="T13">
         <v>19.899999999999999</v>
       </c>
-      <c r="O13">
+      <c r="U13">
         <v>21</v>
       </c>
-      <c r="P13">
+      <c r="V13">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>36</v>
       </c>
       <c r="C14">
         <v>845</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="E14">
         <v>2.5590000000000002</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>934</v>
       </c>
-      <c r="F14">
+      <c r="G14" s="2">
+        <v>0.39861111111111108</v>
+      </c>
+      <c r="H14">
         <v>8.6199999999999992</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>7.3</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>19.8</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>1433</v>
       </c>
-      <c r="J14">
+      <c r="L14" s="2">
+        <v>0.60625000000000007</v>
+      </c>
+      <c r="M14">
         <v>0.95199999999999996</v>
       </c>
-      <c r="K14">
+      <c r="N14">
         <v>1442</v>
       </c>
-      <c r="L14">
+      <c r="O14" s="2">
+        <v>0.61249999999999993</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="1"/>
+        <v>308</v>
+      </c>
+      <c r="R14">
         <v>8.7100000000000009</v>
       </c>
-      <c r="M14">
+      <c r="S14">
         <v>7.4</v>
       </c>
-      <c r="N14">
+      <c r="T14">
         <v>19.8</v>
       </c>
-      <c r="O14">
+      <c r="U14">
         <v>25</v>
       </c>
-      <c r="P14">
+      <c r="V14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="C15">
         <v>850</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="E15">
         <v>8.4559999999999995</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>943</v>
       </c>
-      <c r="F15">
+      <c r="G15" s="2">
+        <v>0.40486111111111112</v>
+      </c>
+      <c r="H15">
         <v>9.9</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>7.3</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>20.3</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>1435</v>
       </c>
-      <c r="J15">
+      <c r="L15" s="2">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="M15">
         <v>5.1310000000000002</v>
       </c>
-      <c r="K15">
+      <c r="N15">
         <v>1445</v>
       </c>
-      <c r="L15">
+      <c r="O15" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" si="0"/>
+        <v>345</v>
+      </c>
+      <c r="Q15" s="4">
+        <f t="shared" si="1"/>
+        <v>302</v>
+      </c>
+      <c r="R15">
         <v>9.4700000000000006</v>
       </c>
-      <c r="M15">
+      <c r="S15">
         <v>7.4</v>
       </c>
-      <c r="N15">
+      <c r="T15">
         <v>19.600000000000001</v>
       </c>
-      <c r="O15">
+      <c r="U15">
         <v>16</v>
       </c>
-      <c r="P15">
+      <c r="V15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
       <c r="C16">
         <v>858</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
+        <v>0.37361111111111112</v>
+      </c>
+      <c r="E16">
         <v>15.11</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>958</v>
       </c>
-      <c r="F16">
+      <c r="G16" s="2">
+        <v>0.4152777777777778</v>
+      </c>
+      <c r="H16">
         <v>11.33</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>7.3</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>20.399999999999999</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>1436</v>
       </c>
-      <c r="J16">
+      <c r="L16" s="2">
+        <v>0.60833333333333328</v>
+      </c>
+      <c r="M16">
         <v>7.54</v>
       </c>
-      <c r="K16">
+      <c r="N16">
         <v>1452</v>
       </c>
-      <c r="L16">
+      <c r="O16" s="2">
+        <v>0.61944444444444446</v>
+      </c>
+      <c r="P16" s="4">
+        <f t="shared" si="0"/>
+        <v>338</v>
+      </c>
+      <c r="Q16" s="4">
+        <f t="shared" si="1"/>
+        <v>294</v>
+      </c>
+      <c r="R16">
         <v>12.82</v>
       </c>
-      <c r="M16">
+      <c r="S16">
         <v>7.4</v>
       </c>
-      <c r="N16">
+      <c r="T16">
         <v>20</v>
       </c>
-      <c r="O16">
+      <c r="U16">
         <v>19</v>
       </c>
-      <c r="P16">
+      <c r="V16">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>29</v>
       </c>
       <c r="C17">
         <v>903</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
+        <v>0.37708333333333338</v>
+      </c>
+      <c r="E17">
         <v>23.5</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>1006</v>
       </c>
-      <c r="F17">
+      <c r="G17" s="2">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="H17">
         <v>12.53</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>7.4</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>20.5</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>1501</v>
       </c>
-      <c r="J17">
+      <c r="L17" s="2">
+        <v>0.62569444444444444</v>
+      </c>
+      <c r="M17">
         <v>11.91</v>
       </c>
-      <c r="K17">
+      <c r="N17">
         <v>1505</v>
       </c>
-      <c r="L17">
+      <c r="O17" s="2">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="P17" s="4">
+        <f t="shared" si="0"/>
+        <v>358</v>
+      </c>
+      <c r="Q17" s="4">
+        <f t="shared" si="1"/>
+        <v>299</v>
+      </c>
+      <c r="R17">
         <v>11.67</v>
       </c>
-      <c r="M17">
+      <c r="S17">
         <v>7.4</v>
       </c>
-      <c r="N17">
+      <c r="T17">
         <v>19</v>
       </c>
-      <c r="O17">
+      <c r="U17">
         <v>20</v>
       </c>
-      <c r="P17">
+      <c r="V17">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>33</v>
       </c>
       <c r="C18">
         <v>912</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="E18">
         <v>2.8809999999999998</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>1010</v>
       </c>
-      <c r="F18">
+      <c r="G18" s="2">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="H18">
         <v>9.9700000000000006</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>7.3</v>
       </c>
-      <c r="H18">
+      <c r="J18">
         <v>19.600000000000001</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>1503</v>
       </c>
-      <c r="J18">
+      <c r="L18" s="2">
+        <v>0.62708333333333333</v>
+      </c>
+      <c r="M18">
         <v>1.45</v>
       </c>
-      <c r="K18">
+      <c r="N18">
         <v>1509</v>
       </c>
-      <c r="L18">
+      <c r="O18" s="2">
+        <v>0.63124999999999998</v>
+      </c>
+      <c r="P18" s="4">
+        <f t="shared" si="0"/>
+        <v>351</v>
+      </c>
+      <c r="Q18" s="4">
+        <f t="shared" si="1"/>
+        <v>299</v>
+      </c>
+      <c r="R18">
         <v>8.56</v>
       </c>
-      <c r="M18">
+      <c r="S18">
         <v>7.5</v>
       </c>
-      <c r="N18">
+      <c r="T18">
         <v>20.5</v>
       </c>
-      <c r="O18">
+      <c r="U18">
         <v>26</v>
       </c>
-      <c r="P18">
+      <c r="V18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
       <c r="C19">
         <v>916</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
+        <v>0.38611111111111113</v>
+      </c>
+      <c r="E19">
         <v>7.9260000000000002</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>1016</v>
       </c>
-      <c r="F19">
+      <c r="G19" s="2">
+        <v>0.42777777777777781</v>
+      </c>
+      <c r="H19">
         <v>9.98</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>7.4</v>
       </c>
-      <c r="H19">
+      <c r="J19">
         <v>19.3</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <v>1506</v>
       </c>
-      <c r="J19">
+      <c r="L19" s="2">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="M19">
         <v>5.6289999999999996</v>
       </c>
-      <c r="K19">
+      <c r="N19">
         <v>1516</v>
       </c>
-      <c r="L19">
+      <c r="O19" s="2">
+        <v>0.63611111111111118</v>
+      </c>
+      <c r="P19" s="4">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="Q19" s="4">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="R19">
         <v>9.1999999999999993</v>
       </c>
-      <c r="M19">
+      <c r="S19">
         <v>7.4</v>
       </c>
-      <c r="N19">
+      <c r="T19">
         <v>20.2</v>
       </c>
-      <c r="O19">
+      <c r="U19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
       <c r="C20">
         <v>922</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
+        <v>0.39027777777777778</v>
+      </c>
+      <c r="E20">
         <v>14.96</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>1023</v>
       </c>
-      <c r="F20">
+      <c r="G20" s="2">
+        <v>0.43263888888888885</v>
+      </c>
+      <c r="H20">
         <v>15.34</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>7.4</v>
       </c>
-      <c r="H20">
+      <c r="J20">
         <v>19.399999999999999</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <v>1507</v>
       </c>
-      <c r="J20">
+      <c r="L20" s="2">
+        <v>0.62986111111111109</v>
+      </c>
+      <c r="M20">
         <v>5.0599999999999996</v>
       </c>
-      <c r="K20">
+      <c r="N20">
         <v>1528</v>
       </c>
-      <c r="L20">
+      <c r="O20" s="2">
+        <v>0.64444444444444449</v>
+      </c>
+      <c r="P20" s="4">
+        <f t="shared" si="0"/>
+        <v>345</v>
+      </c>
+      <c r="Q20" s="4">
+        <f t="shared" si="1"/>
+        <v>305</v>
+      </c>
+      <c r="R20">
         <v>14.79</v>
       </c>
-      <c r="M20">
+      <c r="S20">
         <v>7.5</v>
       </c>
-      <c r="N20">
+      <c r="T20">
         <v>20.2</v>
       </c>
-      <c r="O20">
+      <c r="U20">
         <v>11</v>
       </c>
-      <c r="P20">
+      <c r="V20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>22</v>
       </c>
       <c r="C21">
         <v>925</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="E21">
         <v>0.92700000000000005</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>1028</v>
       </c>
-      <c r="F21">
+      <c r="G21" s="2">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="H21">
         <v>7.41</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>7.4</v>
       </c>
-      <c r="H21">
+      <c r="J21">
         <v>19.600000000000001</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>1513</v>
       </c>
-      <c r="J21">
+      <c r="L21" s="2">
+        <v>0.63402777777777775</v>
+      </c>
+      <c r="M21">
         <v>0.91500000000000004</v>
       </c>
-      <c r="K21">
+      <c r="N21">
         <v>1536</v>
       </c>
-      <c r="L21">
+      <c r="O21" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="P21" s="4">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+      <c r="Q21" s="4">
+        <f t="shared" si="1"/>
+        <v>308</v>
+      </c>
+      <c r="R21">
         <v>7.72</v>
       </c>
-      <c r="M21">
+      <c r="S21">
         <v>7.5</v>
       </c>
-      <c r="N21">
+      <c r="T21">
         <v>20.399999999999999</v>
       </c>
-      <c r="O21">
+      <c r="U21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>34</v>
       </c>
       <c r="C22">
         <v>933</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
+        <v>0.3979166666666667</v>
+      </c>
+      <c r="E22">
         <v>2.6480000000000001</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>1033</v>
       </c>
-      <c r="F22">
+      <c r="G22" s="2">
+        <v>0.43958333333333338</v>
+      </c>
+      <c r="H22">
         <v>8.42</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>7.4</v>
       </c>
-      <c r="H22">
+      <c r="J22">
         <v>19.5</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <v>1533</v>
       </c>
-      <c r="J22">
+      <c r="L22" s="2">
+        <v>0.6479166666666667</v>
+      </c>
+      <c r="M22">
         <v>1.1559999999999999</v>
       </c>
-      <c r="K22">
+      <c r="N22">
         <v>1538</v>
       </c>
-      <c r="L22">
+      <c r="O22" s="2">
+        <v>0.65138888888888891</v>
+      </c>
+      <c r="P22" s="4">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="Q22" s="4">
+        <f t="shared" si="1"/>
+        <v>305</v>
+      </c>
+      <c r="R22">
         <v>8.3699999999999992</v>
       </c>
-      <c r="M22">
+      <c r="S22">
         <v>7.4</v>
       </c>
-      <c r="N22">
+      <c r="T22">
         <v>20.2</v>
       </c>
-      <c r="O22">
+      <c r="U22">
         <v>18</v>
       </c>
-      <c r="P22">
+      <c r="V22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
       <c r="C23">
         <v>941</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
+        <v>0.40347222222222223</v>
+      </c>
+      <c r="E23">
         <v>8.1340000000000003</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>1036</v>
       </c>
-      <c r="F23">
+      <c r="G23" s="2">
+        <v>0.44166666666666665</v>
+      </c>
+      <c r="H23">
         <v>9.61</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <v>7.3</v>
       </c>
-      <c r="H23">
+      <c r="J23">
         <v>19.8</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>1535</v>
       </c>
-      <c r="J23">
+      <c r="L23" s="2">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="M23">
         <v>6.12</v>
       </c>
-      <c r="K23">
+      <c r="N23">
         <v>1544</v>
       </c>
-      <c r="L23">
+      <c r="O23" s="2">
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="P23" s="4">
+        <f t="shared" si="0"/>
+        <v>354</v>
+      </c>
+      <c r="Q23" s="4">
+        <f t="shared" si="1"/>
+        <v>308</v>
+      </c>
+      <c r="R23">
         <v>12.26</v>
       </c>
-      <c r="M23">
+      <c r="S23">
         <v>7.4</v>
       </c>
-      <c r="N23">
+      <c r="T23">
         <v>20.100000000000001</v>
       </c>
-      <c r="O23">
+      <c r="U23">
         <v>18</v>
       </c>
-      <c r="P23">
+      <c r="V23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>14</v>
       </c>
       <c r="C24">
         <v>945</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="E24">
         <v>14.11</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>1047</v>
       </c>
-      <c r="F24">
+      <c r="G24" s="2">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="H24">
         <v>10.08</v>
       </c>
-      <c r="G24">
+      <c r="I24">
         <v>7.5</v>
       </c>
-      <c r="H24">
+      <c r="J24">
         <v>19.5</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <v>1537</v>
       </c>
-      <c r="J24">
+      <c r="L24" s="2">
+        <v>0.65069444444444446</v>
+      </c>
+      <c r="M24">
         <v>16.05</v>
       </c>
-      <c r="K24">
+      <c r="N24">
         <v>1550</v>
       </c>
-      <c r="L24">
+      <c r="O24" s="2">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="P24" s="4">
+        <f t="shared" si="0"/>
+        <v>352</v>
+      </c>
+      <c r="Q24" s="4">
+        <f t="shared" si="1"/>
+        <v>303</v>
+      </c>
+      <c r="R24">
         <v>11.31</v>
       </c>
-      <c r="M24">
+      <c r="S24">
         <v>7.5</v>
       </c>
-      <c r="N24">
+      <c r="T24">
         <v>20.399999999999999</v>
       </c>
-      <c r="O24">
+      <c r="U24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>19</v>
       </c>
       <c r="C25">
         <v>952</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
+        <v>0.41111111111111115</v>
+      </c>
+      <c r="E25">
         <v>0.81799999999999995</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>1051</v>
       </c>
-      <c r="F25">
+      <c r="G25" s="2">
+        <v>0.45208333333333334</v>
+      </c>
+      <c r="H25">
         <v>9.18</v>
       </c>
-      <c r="G25">
+      <c r="I25">
         <v>7.4</v>
       </c>
-      <c r="H25">
+      <c r="J25">
         <v>19.5</v>
       </c>
-      <c r="I25">
+      <c r="K25">
         <v>1539</v>
       </c>
-      <c r="J25">
+      <c r="L25" s="2">
+        <v>0.65208333333333335</v>
+      </c>
+      <c r="M25">
         <v>0.81200000000000006</v>
       </c>
-      <c r="K25">
+      <c r="N25">
         <v>1602</v>
       </c>
-      <c r="L25">
+      <c r="O25" s="2">
+        <v>0.66805555555555562</v>
+      </c>
+      <c r="P25" s="4">
+        <f t="shared" si="0"/>
+        <v>347</v>
+      </c>
+      <c r="Q25" s="4">
+        <f t="shared" si="1"/>
+        <v>311</v>
+      </c>
+      <c r="R25">
         <v>9.25</v>
       </c>
-      <c r="M25">
+      <c r="S25">
         <v>7.4</v>
       </c>
-      <c r="N25">
+      <c r="T25">
         <v>20.5</v>
       </c>
-      <c r="O25">
+      <c r="U25">
         <v>30</v>
       </c>
-      <c r="P25">
+      <c r="V25">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>30</v>
       </c>
       <c r="C26">
         <v>957</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="E26">
         <v>21.34</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>1058</v>
       </c>
-      <c r="F26">
+      <c r="G26" s="2">
+        <v>0.45694444444444443</v>
+      </c>
+      <c r="H26">
         <v>12.52</v>
       </c>
-      <c r="G26">
+      <c r="I26">
         <v>7.5</v>
       </c>
-      <c r="H26">
+      <c r="J26">
         <v>19.8</v>
       </c>
-      <c r="I26">
+      <c r="K26">
         <v>1540</v>
       </c>
-      <c r="J26">
+      <c r="L26" s="2">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="M26">
         <v>19.489999999999998</v>
       </c>
-      <c r="K26">
+      <c r="N26">
         <v>1616</v>
       </c>
-      <c r="L26">
+      <c r="O26" s="2">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="P26" s="4">
+        <f t="shared" si="0"/>
+        <v>343</v>
+      </c>
+      <c r="Q26" s="4">
+        <f t="shared" si="1"/>
+        <v>318</v>
+      </c>
+      <c r="R26">
         <v>13.03</v>
       </c>
-      <c r="M26">
+      <c r="S26">
         <v>7.5</v>
       </c>
-      <c r="N26">
+      <c r="T26">
         <v>20.5</v>
       </c>
-      <c r="O26">
+      <c r="U26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5</v>
       </c>
       <c r="C27">
         <v>1034</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="E27">
         <v>8.9139999999999997</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>1100</v>
       </c>
-      <c r="F27">
+      <c r="G27" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H27">
         <v>10.62</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <v>7.5</v>
       </c>
-      <c r="H27">
+      <c r="J27">
         <v>19.399999999999999</v>
       </c>
-      <c r="I27">
+      <c r="K27">
         <v>1633</v>
       </c>
-      <c r="J27">
+      <c r="L27" s="2">
+        <v>0.68958333333333333</v>
+      </c>
+      <c r="M27">
         <v>8.2530000000000001</v>
       </c>
-      <c r="K27">
+      <c r="N27">
         <v>1638</v>
       </c>
-      <c r="L27">
+      <c r="O27" s="2">
+        <v>0.69305555555555554</v>
+      </c>
+      <c r="P27" s="4">
+        <f t="shared" si="0"/>
+        <v>359</v>
+      </c>
+      <c r="Q27" s="4">
+        <f t="shared" si="1"/>
+        <v>338</v>
+      </c>
+      <c r="R27">
         <v>8.7799999999999994</v>
       </c>
-      <c r="M27">
+      <c r="S27">
         <v>7.4</v>
       </c>
-      <c r="N27">
+      <c r="T27">
         <v>20.3</v>
       </c>
-      <c r="O27">
+      <c r="U27">
         <v>17</v>
       </c>
-      <c r="P27">
+      <c r="V27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>15</v>
       </c>
       <c r="C28">
         <v>1037</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="E28">
         <v>14.19</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>1106</v>
       </c>
-      <c r="F28">
+      <c r="G28" s="2">
+        <v>0.46249999999999997</v>
+      </c>
+      <c r="H28">
         <v>10.41</v>
       </c>
-      <c r="G28">
+      <c r="I28">
         <v>7.6</v>
       </c>
-      <c r="H28">
+      <c r="J28">
         <v>19.7</v>
       </c>
-      <c r="I28">
+      <c r="K28">
         <v>1635</v>
       </c>
-      <c r="J28">
+      <c r="L28" s="2">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="M28">
         <v>13.01</v>
       </c>
-      <c r="K28">
+      <c r="N28">
         <v>1642</v>
       </c>
-      <c r="L28">
+      <c r="O28" s="2">
+        <v>0.6958333333333333</v>
+      </c>
+      <c r="P28" s="4">
+        <f t="shared" si="0"/>
+        <v>358</v>
+      </c>
+      <c r="Q28" s="4">
+        <f t="shared" si="1"/>
+        <v>336</v>
+      </c>
+      <c r="R28">
         <v>10.39</v>
       </c>
-      <c r="M28">
+      <c r="S28">
         <v>7.5</v>
       </c>
-      <c r="N28">
+      <c r="T28">
         <v>20.100000000000001</v>
       </c>
-      <c r="O28">
+      <c r="U28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>21</v>
       </c>
       <c r="C30">
         <v>1045</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E30">
         <v>0.872</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>1122</v>
       </c>
-      <c r="F30">
+      <c r="G30" s="2">
+        <v>0.47361111111111115</v>
+      </c>
+      <c r="H30">
         <v>9.5500000000000007</v>
       </c>
-      <c r="G30">
+      <c r="I30">
         <v>7.5</v>
       </c>
-      <c r="H30">
+      <c r="J30">
         <v>19.5</v>
       </c>
-      <c r="I30">
+      <c r="K30">
         <v>1636</v>
       </c>
-      <c r="J30">
+      <c r="L30" s="2">
+        <v>0.69166666666666676</v>
+      </c>
+      <c r="M30">
         <v>0.82799999999999996</v>
       </c>
-      <c r="K30">
+      <c r="N30">
         <v>1655</v>
       </c>
-      <c r="L30">
+      <c r="O30" s="2">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="P30" s="4">
+        <f t="shared" si="0"/>
+        <v>351</v>
+      </c>
+      <c r="Q30" s="4">
+        <f t="shared" si="1"/>
+        <v>333</v>
+      </c>
+      <c r="R30">
         <v>10.42</v>
       </c>
-      <c r="M30">
+      <c r="S30">
         <v>7.5</v>
       </c>
-      <c r="N30">
+      <c r="T30">
         <v>20.100000000000001</v>
       </c>
-      <c r="O30">
+      <c r="U30">
         <v>18</v>
       </c>
-      <c r="P30">
+      <c r="V30">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>26</v>
       </c>
       <c r="C31">
         <v>1053</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
+        <v>0.45347222222222222</v>
+      </c>
+      <c r="E31">
         <v>23.61</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>1125</v>
       </c>
-      <c r="F31">
+      <c r="G31" s="2">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="H31">
         <v>11.41</v>
       </c>
-      <c r="G31">
+      <c r="I31">
         <v>7.5</v>
       </c>
-      <c r="H31">
+      <c r="J31">
         <v>19.8</v>
       </c>
-      <c r="I31">
+      <c r="K31">
         <v>1641</v>
       </c>
-      <c r="J31">
+      <c r="L31" s="2">
+        <v>0.69513888888888886</v>
+      </c>
+      <c r="M31">
         <v>6.0880000000000001</v>
       </c>
-      <c r="K31">
+      <c r="N31">
         <v>1602</v>
       </c>
-      <c r="L31">
+      <c r="O31" s="2">
+        <v>0.66805555555555562</v>
+      </c>
+      <c r="P31" s="4">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+      <c r="Q31" s="4">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+      <c r="R31">
         <v>13.04</v>
       </c>
-      <c r="M31">
+      <c r="S31">
         <v>7.4</v>
       </c>
-      <c r="N31">
+      <c r="T31">
         <v>20.100000000000001</v>
       </c>
-      <c r="O31">
+      <c r="U31">
         <v>29</v>
       </c>
-      <c r="P31">
+      <c r="V31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>39</v>
       </c>
       <c r="C32">
         <v>1056</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
+        <v>0.45555555555555555</v>
+      </c>
+      <c r="E32">
         <v>2.5230000000000001</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>1134</v>
       </c>
-      <c r="F32">
+      <c r="G32" s="2">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="H32">
         <v>10.94</v>
       </c>
-      <c r="G32">
+      <c r="I32">
         <v>7.5</v>
       </c>
-      <c r="H32">
+      <c r="J32">
         <v>20</v>
       </c>
-      <c r="I32">
+      <c r="K32">
         <v>1643</v>
       </c>
-      <c r="J32">
+      <c r="L32" s="2">
+        <v>0.69652777777777775</v>
+      </c>
+      <c r="M32">
         <v>1.849</v>
       </c>
-      <c r="K32">
+      <c r="N32">
         <v>1710</v>
       </c>
-      <c r="L32">
+      <c r="O32" s="2">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="P32" s="4">
+        <f t="shared" si="0"/>
+        <v>347</v>
+      </c>
+      <c r="Q32" s="4">
+        <f t="shared" si="1"/>
+        <v>336</v>
+      </c>
+      <c r="R32">
         <v>9.57</v>
       </c>
-      <c r="M32">
+      <c r="S32">
         <v>7.5</v>
       </c>
-      <c r="N32">
+      <c r="T32">
         <v>20</v>
       </c>
-      <c r="O32">
+      <c r="U32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9</v>
       </c>
       <c r="C33">
         <v>1112</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
+        <v>0.46666666666666662</v>
+      </c>
+      <c r="E33">
         <v>13.97</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>1139</v>
       </c>
-      <c r="F33">
+      <c r="G33" s="2">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="H33">
         <v>10.1</v>
       </c>
-      <c r="G33">
+      <c r="I33">
         <v>7.4</v>
       </c>
-      <c r="H33">
+      <c r="J33">
         <v>20.399999999999999</v>
       </c>
-      <c r="I33">
+      <c r="K33">
         <v>1711</v>
       </c>
-      <c r="J33">
+      <c r="L33" s="2">
+        <v>0.71597222222222223</v>
+      </c>
+      <c r="M33">
         <v>8.3559999999999999</v>
       </c>
-      <c r="K33">
+      <c r="N33">
         <v>1723</v>
       </c>
-      <c r="L33">
+      <c r="O33" s="2">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="P33" s="4">
+        <f t="shared" si="0"/>
+        <v>359</v>
+      </c>
+      <c r="Q33" s="4">
+        <f t="shared" si="1"/>
+        <v>344</v>
+      </c>
+      <c r="R33">
         <v>13.42</v>
       </c>
-      <c r="M33">
+      <c r="S33">
         <v>7.5</v>
       </c>
-      <c r="N33">
+      <c r="T33">
         <v>19.899999999999999</v>
       </c>
-      <c r="O33">
+      <c r="U33">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>24</v>
       </c>
       <c r="C34">
         <v>1116</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
+        <v>0.4694444444444445</v>
+      </c>
+      <c r="E34">
         <v>0.90600000000000003</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>1145</v>
       </c>
-      <c r="F34">
+      <c r="G34" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="H34">
         <v>7.28</v>
       </c>
-      <c r="G34">
+      <c r="I34">
         <v>7.4</v>
       </c>
-      <c r="H34">
+      <c r="J34">
         <v>20.399999999999999</v>
       </c>
-      <c r="I34">
+      <c r="K34">
         <v>1713</v>
       </c>
-      <c r="J34">
+      <c r="L34" s="2">
+        <v>0.71736111111111101</v>
+      </c>
+      <c r="M34">
         <v>0.95199999999999996</v>
       </c>
-      <c r="K34">
+      <c r="N34">
         <v>1726</v>
       </c>
-      <c r="L34">
+      <c r="O34" s="2">
+        <v>0.72638888888888886</v>
+      </c>
+      <c r="P34" s="4">
+        <f t="shared" si="0"/>
+        <v>357</v>
+      </c>
+      <c r="Q34" s="4">
+        <f t="shared" si="1"/>
+        <v>341</v>
+      </c>
+      <c r="R34">
         <v>7.7</v>
       </c>
-      <c r="M34">
+      <c r="S34">
         <v>7.5</v>
       </c>
-      <c r="N34">
+      <c r="T34">
         <v>20.2</v>
       </c>
-      <c r="O34">
+      <c r="U34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
       <c r="C35">
         <v>1120</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E35">
         <v>22.18</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>1155</v>
       </c>
-      <c r="F35">
+      <c r="G35" s="2">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="H35">
         <v>11.41</v>
       </c>
-      <c r="G35">
+      <c r="I35">
         <v>7.6</v>
       </c>
-      <c r="H35">
+      <c r="J35">
         <v>20</v>
       </c>
-      <c r="I35">
+      <c r="K35">
         <v>1714</v>
       </c>
-      <c r="J35">
+      <c r="L35" s="2">
+        <v>0.71805555555555556</v>
+      </c>
+      <c r="M35">
         <v>18.97</v>
       </c>
-      <c r="K35">
+      <c r="N35">
         <v>1732</v>
       </c>
-      <c r="L35">
+      <c r="O35" s="2">
+        <v>0.73055555555555562</v>
+      </c>
+      <c r="P35" s="4">
+        <f t="shared" si="0"/>
+        <v>354</v>
+      </c>
+      <c r="Q35" s="4">
+        <f t="shared" si="1"/>
+        <v>337</v>
+      </c>
+      <c r="R35">
         <v>11.56</v>
       </c>
-      <c r="M35">
+      <c r="S35">
         <v>7.5</v>
       </c>
-      <c r="N35">
+      <c r="T35">
         <v>20.3</v>
       </c>
-      <c r="O35">
+      <c r="U35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7</v>
       </c>
       <c r="C36">
         <v>1130</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E36">
         <v>8.4420000000000002</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>1158</v>
       </c>
-      <c r="F36">
+      <c r="G36" s="2">
+        <v>0.49861111111111112</v>
+      </c>
+      <c r="H36">
         <v>9.27</v>
       </c>
-      <c r="G36">
+      <c r="I36">
         <v>7.6</v>
       </c>
-      <c r="H36">
+      <c r="J36">
         <v>19.600000000000001</v>
       </c>
-      <c r="I36">
+      <c r="K36">
         <v>1716</v>
       </c>
-      <c r="J36">
+      <c r="L36" s="2">
+        <v>0.71944444444444444</v>
+      </c>
+      <c r="M36">
         <v>8.6620000000000008</v>
       </c>
-      <c r="K36">
+      <c r="N36">
         <v>1743</v>
       </c>
-      <c r="L36">
+      <c r="O36" s="2">
+        <v>0.73819444444444438</v>
+      </c>
+      <c r="P36" s="4">
+        <f t="shared" si="0"/>
+        <v>346</v>
+      </c>
+      <c r="Q36" s="4">
+        <f t="shared" si="1"/>
+        <v>345</v>
+      </c>
+      <c r="R36">
         <v>10.26</v>
       </c>
-      <c r="M36">
+      <c r="S36">
         <v>7.6</v>
       </c>
-      <c r="N36">
+      <c r="T36">
         <v>20.399999999999999</v>
       </c>
-      <c r="O36">
+      <c r="U36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>32</v>
       </c>
       <c r="C37">
         <v>1136</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="E37">
         <v>21.18</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>1209</v>
       </c>
-      <c r="F37">
+      <c r="G37" s="2">
+        <v>0.50624999999999998</v>
+      </c>
+      <c r="H37">
         <v>15.67</v>
       </c>
-      <c r="G37">
+      <c r="I37">
         <v>7.7</v>
       </c>
-      <c r="H37">
+      <c r="J37">
         <v>20.100000000000001</v>
       </c>
-      <c r="I37">
+      <c r="K37">
         <v>1718</v>
       </c>
-      <c r="J37">
+      <c r="L37" s="2">
+        <v>0.72083333333333333</v>
+      </c>
+      <c r="M37">
         <v>20.89</v>
       </c>
-      <c r="K37">
+      <c r="N37">
         <v>1753</v>
       </c>
-      <c r="L37">
+      <c r="O37" s="2">
+        <v>0.74513888888888891</v>
+      </c>
+      <c r="P37" s="4">
+        <f t="shared" si="0"/>
+        <v>342</v>
+      </c>
+      <c r="Q37" s="4">
+        <f t="shared" si="1"/>
+        <v>344</v>
+      </c>
+      <c r="R37">
         <v>15.95</v>
       </c>
-      <c r="M37">
+      <c r="S37">
         <v>7.6</v>
       </c>
-      <c r="N37">
+      <c r="T37">
         <v>20.100000000000001</v>
       </c>
-      <c r="O37">
+      <c r="U37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>40</v>
       </c>
       <c r="C38">
         <v>1140</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="E38">
         <v>2.82</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>1216</v>
       </c>
-      <c r="F38">
+      <c r="G38" s="2">
+        <v>0.51111111111111118</v>
+      </c>
+      <c r="H38">
         <v>7.82</v>
       </c>
-      <c r="G38">
+      <c r="I38">
         <v>7.6</v>
       </c>
-      <c r="H38">
+      <c r="J38">
         <v>19.600000000000001</v>
       </c>
-      <c r="I38">
+      <c r="K38">
         <v>1740</v>
       </c>
-      <c r="J38">
+      <c r="L38" s="2">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="M38">
         <v>2.032</v>
       </c>
-      <c r="K38">
+      <c r="N38">
         <v>1800</v>
       </c>
-      <c r="L38">
+      <c r="O38" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="P38" s="4">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="Q38" s="4">
+        <f t="shared" si="1"/>
+        <v>344</v>
+      </c>
+      <c r="R38">
         <v>8.16</v>
       </c>
-      <c r="M38">
+      <c r="S38">
         <v>7.6</v>
       </c>
-      <c r="N38">
+      <c r="T38">
         <v>20.3</v>
       </c>
-      <c r="O38">
+      <c r="U38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8</v>
       </c>
       <c r="C39">
         <v>1146</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="2">
+        <v>0.49027777777777781</v>
+      </c>
+      <c r="E39">
         <v>8.1340000000000003</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>1227</v>
       </c>
-      <c r="F39">
+      <c r="G39" s="2">
+        <v>0.51874999999999993</v>
+      </c>
+      <c r="H39">
         <v>11.63</v>
       </c>
-      <c r="G39">
+      <c r="I39">
         <v>7.6</v>
       </c>
-      <c r="H39">
+      <c r="J39">
         <v>19.5</v>
       </c>
-      <c r="I39">
+      <c r="K39">
         <v>1741</v>
       </c>
-      <c r="J39">
+      <c r="L39" s="2">
+        <v>0.7368055555555556</v>
+      </c>
+      <c r="M39">
         <v>7.51</v>
       </c>
-      <c r="K39">
+      <c r="N39">
         <v>1816</v>
       </c>
-      <c r="L39">
+      <c r="O39" s="2">
+        <v>0.76111111111111107</v>
+      </c>
+      <c r="P39" s="4">
+        <f t="shared" si="0"/>
+        <v>355</v>
+      </c>
+      <c r="Q39" s="4">
+        <f t="shared" si="1"/>
+        <v>349</v>
+      </c>
+      <c r="R39">
         <v>11.36</v>
       </c>
-      <c r="M39">
+      <c r="S39">
         <v>7.5</v>
       </c>
-      <c r="N39">
+      <c r="T39">
         <v>20</v>
       </c>
-      <c r="O39">
+      <c r="U39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
       <c r="C40">
         <v>1153</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
+        <v>0.49513888888888885</v>
+      </c>
+      <c r="E40">
         <v>2.544</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>1231</v>
       </c>
-      <c r="F40">
+      <c r="G40" s="2">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="H40">
         <v>10.55</v>
       </c>
-      <c r="G40">
+      <c r="I40">
         <v>7.5</v>
       </c>
-      <c r="H40">
+      <c r="J40">
         <v>19.899999999999999</v>
       </c>
-      <c r="I40">
+      <c r="K40">
         <v>1744</v>
       </c>
-      <c r="J40">
+      <c r="L40" s="2">
+        <v>0.73888888888888893</v>
+      </c>
+      <c r="M40">
         <v>1.429</v>
       </c>
-      <c r="K40">
+      <c r="N40">
         <v>1822</v>
       </c>
-      <c r="L40">
+      <c r="O40" s="2">
+        <v>0.76527777777777783</v>
+      </c>
+      <c r="P40" s="4">
+        <f t="shared" si="0"/>
+        <v>351</v>
+      </c>
+      <c r="Q40" s="4">
+        <f t="shared" si="1"/>
+        <v>351</v>
+      </c>
+      <c r="R40">
         <v>8.82</v>
       </c>
-      <c r="M40">
+      <c r="S40">
         <v>7.5</v>
       </c>
-      <c r="N40">
+      <c r="T40">
         <v>19.8</v>
       </c>
-      <c r="O40">
+      <c r="U40">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>16</v>
       </c>
       <c r="C41">
         <v>1215</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E41">
         <v>13.32</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>1236</v>
       </c>
-      <c r="F41">
+      <c r="G41" s="2">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="H41">
         <v>12.97</v>
       </c>
-      <c r="G41">
+      <c r="I41">
         <v>7.6</v>
       </c>
-      <c r="H41">
+      <c r="J41">
         <v>20.100000000000001</v>
       </c>
-      <c r="I41">
+      <c r="K41">
         <v>1745</v>
       </c>
-      <c r="J41">
+      <c r="L41" s="2">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="M41">
         <v>13.98</v>
       </c>
-      <c r="K41">
+      <c r="N41">
         <v>1836</v>
       </c>
-      <c r="L41">
+      <c r="O41" s="2">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="P41" s="4">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+      <c r="Q41" s="4">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+      <c r="R41">
         <v>12.66</v>
       </c>
-      <c r="M41">
+      <c r="S41">
         <v>7.6</v>
       </c>
-      <c r="N41">
+      <c r="T41">
         <v>20</v>
       </c>
-      <c r="O41">
+      <c r="U41">
         <v>0</v>
       </c>
     </row>

</xml_diff>